<commit_message>
dataframe timespeciific for correlations
</commit_message>
<xml_diff>
--- a/data_analysis/manuale_simulazioni.xlsx
+++ b/data_analysis/manuale_simulazioni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocpa\OneDrive\Documenti\GitHub\watchyouragent\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712931E5-AE65-42F9-8DBA-ED6058E7F87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1FF54F-2768-45D4-858E-EAB37D008876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C49FA2A2-CDCD-4370-A73E-6E8EEDB8A6D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C49FA2A2-CDCD-4370-A73E-6E8EEDB8A6D1}"/>
   </bookViews>
   <sheets>
     <sheet name="simulations_scripts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>variable</t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t>default: muccheslider1, ccr 0  [from above]</t>
+  </si>
+  <si>
+    <t>nrgacqweek</t>
+  </si>
+  <si>
+    <t>newnrgweek</t>
+  </si>
+  <si>
+    <t>energy acquired in that week (last day of week before - last day of the reference week)</t>
+  </si>
+  <si>
+    <t>energy renewed for that week (ccr * 10 of the first day of the reference week)</t>
   </si>
 </sst>
 </file>
@@ -199,10 +211,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -538,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799EB076-ABEA-4D6A-8328-D183D6CC25E1}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,6 +664,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -660,15 +687,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15946D7-5104-47D3-AF5E-605C3705CDC0}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -676,7 +703,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -687,7 +714,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -698,7 +725,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -706,7 +733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -714,7 +741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -722,7 +749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -730,7 +757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -738,30 +765,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>1</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -769,7 +795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -777,7 +803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -785,7 +811,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -793,7 +819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -801,11 +827,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>2</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>14</v>
       </c>
       <c r="C16" t="s">
@@ -864,10 +890,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>3</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>21</v>
       </c>
       <c r="C23" t="s">
@@ -926,10 +952,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>4</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>28</v>
       </c>
       <c r="C30" t="s">
@@ -988,10 +1014,10 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>5</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>35</v>
       </c>
       <c r="C37" t="s">

</xml_diff>